<commit_message>
trend & moving averages
</commit_message>
<xml_diff>
--- a/Etude de tendance/Etude de tendance PIB Belgique&RFA.xlsx
+++ b/Etude de tendance/Etude de tendance PIB Belgique&RFA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\Time-Series-Analysis\Etude de tendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C977AF2-3529-4F54-AAD5-46AC35E580CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09283E70-53BB-4376-B848-30F14384009F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5460" yWindow="3390" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -173,11 +173,13 @@
       <sz val="10"/>
       <color indexed="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -193,6 +195,7 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -626,7 +629,7 @@
   <dimension ref="A1:Y53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1061,6 +1064,10 @@
         <f>_xlfn.VAR.P(A6:A13)</f>
         <v>5.25</v>
       </c>
+      <c r="K15">
+        <f>_xlfn.COVARIANCE.P(A6:A13,E6:E13)</f>
+        <v>0.71704059472459292</v>
+      </c>
     </row>
     <row r="16" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="10" t="s">

</xml_diff>